<commit_message>
section 2a validation, upload feedback, excel read date problem fixed, section 1 excel read date problem fixed, section 2b upload feedback, section 3 search results query fixed
</commit_message>
<xml_diff>
--- a/docs/Section 1 (Sample Data).xlsx
+++ b/docs/Section 1 (Sample Data).xlsx
@@ -281,11 +281,11 @@
   </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="A8:K30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.62"/>
@@ -400,6 +400,9 @@
       <c r="A4" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <v>456</v>
+      </c>
       <c r="C4" s="0" t="s">
         <v>28</v>
       </c>

</xml_diff>